<commit_message>
Hutcheson test & heatmap
</commit_message>
<xml_diff>
--- a/botnvarpa_jul_des_2021.xlsx
+++ b/botnvarpa_jul_des_2021.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\competition\MHHI_fish_industry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63AEF6A-C678-4C45-8FD6-9BDFD8CD990C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A3B33302-8FDF-48D6-A3A7-EF5846244EDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="2625" windowWidth="21600" windowHeight="11385" xr2:uid="{D621A2B8-C2BC-46F9-A452-659CA935E620}"/>
+    <workbookView xWindow="17625" yWindow="2625" windowWidth="21075" windowHeight="11385" activeTab="2" xr2:uid="{D621A2B8-C2BC-46F9-A452-659CA935E620}"/>
   </bookViews>
   <sheets>
-    <sheet name="5_flokkar" sheetId="1" r:id="rId1"/>
-    <sheet name="5_ferdir" sheetId="2" r:id="rId2"/>
-    <sheet name="an_eftirlitsmanns" sheetId="3" r:id="rId3"/>
+    <sheet name="botnvarpa_jul_des_2021" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId3"/>
+    <sheet name="5_ferdir" sheetId="2" r:id="rId4"/>
+    <sheet name="an_eftirlitsmanns" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="40">
   <si>
     <t>Þorskur</t>
   </si>
@@ -115,6 +117,45 @@
   </si>
   <si>
     <t>Thorskur</t>
+  </si>
+  <si>
+    <t>names</t>
+  </si>
+  <si>
+    <t>Ýsa</t>
+  </si>
+  <si>
+    <t>Sandkoli</t>
+  </si>
+  <si>
+    <t>Sólkoli</t>
+  </si>
+  <si>
+    <t>Steinbítur</t>
+  </si>
+  <si>
+    <t>Langlúra</t>
+  </si>
+  <si>
+    <t>Lýsa</t>
+  </si>
+  <si>
+    <t>Lúða</t>
+  </si>
+  <si>
+    <t>Skrápflúra</t>
+  </si>
+  <si>
+    <t>Tindaskata</t>
+  </si>
+  <si>
+    <t>Blálanga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hlýri </t>
+  </si>
+  <si>
+    <t>Skötuselur</t>
   </si>
 </sst>
 </file>
@@ -167,10 +208,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
@@ -488,7 +530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C4E3D8-DD13-458D-8B5E-EA8053E3F6FF}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -602,27 +644,45 @@
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+      <c r="A7" s="2">
+        <v>0</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
       <c r="C7" s="2">
         <v>748</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+      <c r="A8" s="2">
+        <v>0</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
       <c r="C8" s="2">
         <v>686</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="2">
+        <v>0</v>
+      </c>
       <c r="B9" s="2">
         <v>39</v>
       </c>
@@ -641,7 +701,9 @@
       <c r="A10" s="2">
         <v>4</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
       <c r="C10" s="2">
         <v>161</v>
       </c>
@@ -681,14 +743,18 @@
       <c r="C12" s="2">
         <v>43</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
       <c r="E12" s="2">
         <v>29</v>
       </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="2">
+        <v>0</v>
+      </c>
       <c r="B13" s="2">
         <v>3</v>
       </c>
@@ -704,25 +770,39 @@
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
+      <c r="A14" s="2">
+        <v>0</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
       <c r="C14" s="2">
         <v>39</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="2">
+        <v>0</v>
+      </c>
       <c r="B15" s="2">
         <v>44</v>
       </c>
       <c r="C15" s="2">
         <v>23</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -732,19 +812,33 @@
       <c r="B16" s="2">
         <v>26</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="2">
+        <v>0</v>
+      </c>
       <c r="B17" s="2">
         <v>1</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -754,11 +848,15 @@
       <c r="B18" s="2">
         <v>319</v>
       </c>
-      <c r="C18" s="2"/>
+      <c r="C18" s="2">
+        <v>0</v>
+      </c>
       <c r="D18" s="2">
         <v>76</v>
       </c>
-      <c r="E18" s="2"/>
+      <c r="E18" s="2">
+        <v>0</v>
+      </c>
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -768,9 +866,15 @@
       <c r="B19" s="2">
         <v>70</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="C19" s="2">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
       <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -779,6 +883,15 @@
       </c>
       <c r="B20" s="2">
         <v>8</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -788,6 +901,727 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E71EC84B-8B43-40B5-BA12-8838253F0B23}">
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="A1:F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1330</v>
+      </c>
+      <c r="C2" s="2">
+        <v>6326</v>
+      </c>
+      <c r="D2" s="2">
+        <v>38353</v>
+      </c>
+      <c r="E2" s="2">
+        <v>5980</v>
+      </c>
+      <c r="F2" s="2">
+        <v>4668</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2">
+        <v>44942</v>
+      </c>
+      <c r="C3" s="2">
+        <v>39093</v>
+      </c>
+      <c r="D3" s="2">
+        <v>11900</v>
+      </c>
+      <c r="E3" s="2">
+        <v>35074</v>
+      </c>
+      <c r="F3" s="2">
+        <v>13896</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2568</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2807</v>
+      </c>
+      <c r="D4" s="2">
+        <v>9636</v>
+      </c>
+      <c r="E4" s="2">
+        <v>9823</v>
+      </c>
+      <c r="F4" s="2">
+        <v>7656</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2">
+        <v>7669</v>
+      </c>
+      <c r="C5" s="2">
+        <v>22914</v>
+      </c>
+      <c r="D5" s="2">
+        <v>8538</v>
+      </c>
+      <c r="E5" s="2">
+        <v>4517</v>
+      </c>
+      <c r="F5" s="2">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2">
+        <v>87</v>
+      </c>
+      <c r="C6" s="2">
+        <v>187</v>
+      </c>
+      <c r="D6" s="2">
+        <v>4295</v>
+      </c>
+      <c r="E6" s="2">
+        <v>160</v>
+      </c>
+      <c r="F6" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>748</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>686</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>39</v>
+      </c>
+      <c r="D9" s="2">
+        <v>272</v>
+      </c>
+      <c r="E9" s="2">
+        <v>100</v>
+      </c>
+      <c r="F9" s="2">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>161</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1167</v>
+      </c>
+      <c r="F10" s="2">
+        <v>2854</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2">
+        <v>181</v>
+      </c>
+      <c r="C11" s="2">
+        <v>304</v>
+      </c>
+      <c r="D11" s="2">
+        <v>56</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1217</v>
+      </c>
+      <c r="F11" s="2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2">
+        <v>19</v>
+      </c>
+      <c r="D12" s="2">
+        <v>43</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
+        <v>3</v>
+      </c>
+      <c r="D13" s="2">
+        <v>40</v>
+      </c>
+      <c r="E13" s="2">
+        <v>101</v>
+      </c>
+      <c r="F13" s="2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
+        <v>39</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2">
+        <v>44</v>
+      </c>
+      <c r="D15" s="2">
+        <v>23</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="2">
+        <v>32</v>
+      </c>
+      <c r="C16" s="2">
+        <v>26</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
+        <v>195</v>
+      </c>
+      <c r="C18" s="2">
+        <v>319</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <v>76</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="2">
+        <v>16</v>
+      </c>
+      <c r="C19" s="2">
+        <v>70</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="2">
+        <v>15</v>
+      </c>
+      <c r="C20" s="2">
+        <v>8</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC7385A-FE88-4C21-9DCD-DF3DCD634790}">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>12607</v>
+      </c>
+      <c r="C2" s="2">
+        <v>16678</v>
+      </c>
+      <c r="D2" s="2">
+        <v>21594</v>
+      </c>
+      <c r="E2" s="2">
+        <v>7181</v>
+      </c>
+      <c r="F2" s="2">
+        <v>39030</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>17109</v>
+      </c>
+      <c r="C3" s="2">
+        <v>11189</v>
+      </c>
+      <c r="D3" s="2">
+        <v>14971</v>
+      </c>
+      <c r="E3" s="2">
+        <v>19020</v>
+      </c>
+      <c r="F3" s="2">
+        <v>15068</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="2">
+        <v>5852</v>
+      </c>
+      <c r="C4" s="2">
+        <v>13539</v>
+      </c>
+      <c r="D4" s="2">
+        <v>12443</v>
+      </c>
+      <c r="E4" s="2">
+        <v>24462</v>
+      </c>
+      <c r="F4" s="2">
+        <v>6035</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2">
+        <v>6491</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1276</v>
+      </c>
+      <c r="D5" s="2">
+        <v>3105</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2537</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1769</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1327</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3193</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2097</v>
+      </c>
+      <c r="E6" s="2">
+        <v>324</v>
+      </c>
+      <c r="F6" s="2">
+        <v>4385</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="2">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="2">
+        <v>326</v>
+      </c>
+      <c r="C8" s="2">
+        <v>563</v>
+      </c>
+      <c r="D8">
+        <v>513</v>
+      </c>
+      <c r="E8" s="2">
+        <v>294</v>
+      </c>
+      <c r="F8" s="2">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9">
+        <v>471</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1071</v>
+      </c>
+      <c r="D9">
+        <v>309</v>
+      </c>
+      <c r="E9">
+        <v>149</v>
+      </c>
+      <c r="F9">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10">
+        <v>285</v>
+      </c>
+      <c r="E10" s="2">
+        <v>64</v>
+      </c>
+      <c r="F10">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>65</v>
+      </c>
+      <c r="C12">
+        <v>107</v>
+      </c>
+      <c r="D12">
+        <v>218</v>
+      </c>
+      <c r="E12">
+        <v>634</v>
+      </c>
+      <c r="F12">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13">
+        <v>41</v>
+      </c>
+      <c r="C13">
+        <v>235</v>
+      </c>
+      <c r="D13">
+        <v>201</v>
+      </c>
+      <c r="E13">
+        <v>39</v>
+      </c>
+      <c r="F13">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="D16">
+        <v>51</v>
+      </c>
+      <c r="E16">
+        <v>98</v>
+      </c>
+      <c r="F16">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB2800C3-4D3C-4CB7-ADDD-9202A13AA180}">
   <dimension ref="A1:T6"/>
   <sheetViews>
@@ -1104,12 +1938,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6076DB76-CD64-4D84-A770-2CD6744622F9}">
   <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>